<commit_message>
Added SAM mock data factory and associated generators.
</commit_message>
<xml_diff>
--- a/docs/data-maps/sam-silver-attr-map.xlsx
+++ b/docs/data-maps/sam-silver-attr-map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\defra\ls-keeper-data-api\docs\data-maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D40098D-4482-4E49-9235-F866FBBA086A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB37A45B-50BC-4822-803C-8EDB08D2EFE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14990" yWindow="40" windowWidth="23580" windowHeight="7840" activeTab="4" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
+    <workbookView xWindow="12280" yWindow="8160" windowWidth="28110" windowHeight="12210" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
   </bookViews>
   <sheets>
     <sheet name="SAM CPHHolding" sheetId="1" r:id="rId1"/>
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="203">
   <si>
     <t>Source</t>
   </si>
@@ -1372,10 +1372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5EF1DC-D2AC-4A4B-82BB-D60D1A15ED0A}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1727,37 +1727,29 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>60</v>
-      </c>
+    <row r="30" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+    </row>
+    <row r="31" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
     </row>
     <row r="32" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="11" t="s">
-        <v>193</v>
+        <v>71</v>
       </c>
       <c r="C32" s="11" t="s">
         <v>96</v>
@@ -1765,109 +1757,115 @@
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
     </row>
-    <row r="33" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="11" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+    </row>
+    <row r="36" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C36" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-    </row>
-    <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="3" t="s">
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+    </row>
+    <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B37" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="E37" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="F37" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="7" t="s">
+    <row r="38" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C38" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8" t="s">
+      <c r="E38" s="8"/>
+      <c r="F38" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="F39" s="5"/>
-    </row>
-    <row r="40" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
+        <v>45</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="41" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="11" t="s">
-        <v>35</v>
+        <v>195</v>
       </c>
       <c r="C41" s="11" t="s">
         <v>96</v>
@@ -1875,15 +1873,47 @@
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
     </row>
-    <row r="42" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="11" t="s">
+    <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A42" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+    </row>
+    <row r="44" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+    </row>
+    <row r="45" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C45" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1896,7 +1926,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2351,7 +2381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B945AFE6-1F03-45E2-947C-33FC1DE5D955}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -2917,8 +2947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D9F3751-E89E-4D65-AA53-4C5E240F65D4}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3493,7 +3523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91CC36E6-DB4D-4568-987C-6F2A58047854}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11:F12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Created support for mocking SAM data for use across all tests (#22)
* Wiring up of the MockSamDataFactory and associated builders.

* Added SAM mock data factory and associated generators.

* Closing file.

* Fixed format linting

* Minor using removal

---------

Co-authored-by: Mark Gent <Mark.Gent@homesengland.gov.uk>
</commit_message>
<xml_diff>
--- a/docs/data-maps/sam-silver-attr-map.xlsx
+++ b/docs/data-maps/sam-silver-attr-map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\defra\ls-keeper-data-api\docs\data-maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D40098D-4482-4E49-9235-F866FBBA086A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8449C433-285A-4E64-BD9E-220258C04D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14990" yWindow="40" windowWidth="23580" windowHeight="7840" activeTab="4" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
+    <workbookView xWindow="9760" yWindow="8070" windowWidth="28110" windowHeight="12210" activeTab="1" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
   </bookViews>
   <sheets>
     <sheet name="SAM CPHHolding" sheetId="1" r:id="rId1"/>
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="203">
   <si>
     <t>Source</t>
   </si>
@@ -1372,10 +1372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5EF1DC-D2AC-4A4B-82BB-D60D1A15ED0A}">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1727,37 +1727,29 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>60</v>
-      </c>
+    <row r="30" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+    </row>
+    <row r="31" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
     </row>
     <row r="32" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="11" t="s">
-        <v>193</v>
+        <v>71</v>
       </c>
       <c r="C32" s="11" t="s">
         <v>96</v>
@@ -1765,109 +1757,115 @@
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
     </row>
-    <row r="33" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="11" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+    </row>
+    <row r="36" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C36" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-    </row>
-    <row r="34" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A34" s="3" t="s">
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+    </row>
+    <row r="37" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B37" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="E37" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="F34" s="5" t="s">
+      <c r="F37" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="7" t="s">
+    <row r="38" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C38" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8" t="s">
+      <c r="E38" s="8"/>
+      <c r="F38" s="8" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A36" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
     </row>
     <row r="39" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="F39" s="5"/>
-    </row>
-    <row r="40" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
+        <v>45</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="41" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="11" t="s">
-        <v>35</v>
+        <v>195</v>
       </c>
       <c r="C41" s="11" t="s">
         <v>96</v>
@@ -1875,15 +1873,47 @@
       <c r="E41" s="12"/>
       <c r="F41" s="12"/>
     </row>
-    <row r="42" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="11" t="s">
+    <row r="42" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A42" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+    </row>
+    <row r="44" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+    </row>
+    <row r="45" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C45" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1895,8 +1925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5113F5DD-FFF9-4DD1-8866-48A257EC0332}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2351,7 +2381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B945AFE6-1F03-45E2-947C-33FC1DE5D955}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -2917,8 +2947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D9F3751-E89E-4D65-AA53-4C5E240F65D4}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3493,7 +3523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91CC36E6-DB4D-4568-987C-6F2A58047854}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11:F12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Sam Holding and Herd silver maps updated.
</commit_message>
<xml_diff>
--- a/docs/data-maps/sam-silver-attr-map.xlsx
+++ b/docs/data-maps/sam-silver-attr-map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\defra\ls-keeper-data-api\docs\data-maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48BCD4E-D633-498D-B255-D21C73C7FE0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06EA7787-16B7-402B-BE67-26BF5EBE1AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1900" windowWidth="24250" windowHeight="15280" activeTab="2" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
+    <workbookView xWindow="-40" yWindow="5600" windowWidth="24250" windowHeight="15280" activeTab="1" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
   </bookViews>
   <sheets>
     <sheet name="SAM CPHHolding" sheetId="1" r:id="rId1"/>
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="260">
   <si>
     <t>Source</t>
   </si>
@@ -710,9 +710,6 @@
     <t>SAON_DESCRIPTION</t>
   </si>
   <si>
-    <t>TO ADD</t>
-  </si>
-  <si>
     <t>FEATURE_NAME *</t>
   </si>
   <si>
@@ -725,9 +722,6 @@
     <t>SECONDARY_CPH *</t>
   </si>
   <si>
-    <t>TO ADD IN AS COMPOSITE KEY</t>
-  </si>
-  <si>
     <t>TO ADD INTO SILVER as Sub Division</t>
   </si>
   <si>
@@ -737,9 +731,6 @@
     <t>ANIMAL_SPECIES_CODE *</t>
   </si>
   <si>
-    <t>TO ADD IN To Help form Gold</t>
-  </si>
-  <si>
     <t>Issue with Data currently</t>
   </si>
   <si>
@@ -800,9 +791,6 @@
     <t>TB-AFU-NA</t>
   </si>
   <si>
-    <t>TO ADD INTO SILVER (may be of use)</t>
-  </si>
-  <si>
     <t>HERDMARK *</t>
   </si>
   <si>
@@ -903,6 +891,21 @@
   </si>
   <si>
     <t>Business</t>
+  </si>
+  <si>
+    <t>SecondaryCph</t>
+  </si>
+  <si>
+    <t>CphRelationshipType</t>
+  </si>
+  <si>
+    <t>PremiseSubActivityTypeCode</t>
+  </si>
+  <si>
+    <t>MovementRestrictionReasonCode</t>
+  </si>
+  <si>
+    <t>ProductionUsageCodeList</t>
   </si>
 </sst>
 </file>
@@ -1121,7 +1124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1189,15 +1192,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1211,13 +1205,7 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1240,28 +1228,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1580,8 +1568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5EF1DC-D2AC-4A4B-82BB-D60D1A15ED0A}">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1705,7 +1693,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="23" t="s">
         <v>125</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1725,8 +1713,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" s="26" t="s">
-        <v>195</v>
+      <c r="A9" s="23" t="s">
+        <v>194</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>11</v>
@@ -1738,10 +1726,10 @@
         <v>59</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -1768,13 +1756,13 @@
       <c r="A11" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="D11" s="32"/>
+      <c r="D11" s="28"/>
       <c r="E11" s="18">
         <v>1</v>
       </c>
@@ -1782,15 +1770,15 @@
         <v>110</v>
       </c>
       <c r="H11" s="16"/>
-      <c r="I11" s="41" t="s">
-        <v>211</v>
+      <c r="I11" s="36" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="F12" s="29"/>
+      <c r="F12" s="26"/>
       <c r="H12" s="20"/>
       <c r="I12" s="21"/>
     </row>
@@ -1801,7 +1789,7 @@
       <c r="E13" s="5">
         <v>3</v>
       </c>
-      <c r="F13" s="29"/>
+      <c r="F13" s="26"/>
       <c r="H13" s="20"/>
       <c r="I13" s="21"/>
     </row>
@@ -1809,22 +1797,20 @@
       <c r="A14" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="F14" s="29"/>
+      <c r="F14" s="26"/>
       <c r="H14" s="20"/>
       <c r="I14" s="21"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="20" t="s">
+    <row r="15" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="37" t="s">
         <v>193</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="F15" s="29"/>
-      <c r="H15" s="20" t="s">
-        <v>209</v>
-      </c>
-      <c r="I15" s="21"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="38"/>
+      <c r="H15" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="I15" s="39"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="20" t="s">
@@ -1833,7 +1819,7 @@
       <c r="E16" s="5">
         <v>10</v>
       </c>
-      <c r="F16" s="29"/>
+      <c r="F16" s="26"/>
       <c r="H16" s="20"/>
       <c r="I16" s="21"/>
     </row>
@@ -1841,7 +1827,7 @@
       <c r="A17" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="F17" s="29"/>
+      <c r="F17" s="26"/>
       <c r="H17" s="20"/>
       <c r="I17" s="21"/>
     </row>
@@ -1852,7 +1838,7 @@
       <c r="E18" s="5">
         <v>12</v>
       </c>
-      <c r="F18" s="29"/>
+      <c r="F18" s="26"/>
       <c r="H18" s="20"/>
       <c r="I18" s="21"/>
     </row>
@@ -1860,25 +1846,23 @@
       <c r="A19" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="F19" s="29"/>
+      <c r="F19" s="26"/>
       <c r="H19" s="20"/>
       <c r="I19" s="21"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="23" t="s">
+    <row r="20" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="40" t="s">
         <v>192</v>
       </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="33" t="s">
-        <v>194</v>
-      </c>
-      <c r="D20" s="33"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="31"/>
-      <c r="H20" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="I20" s="25"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="43"/>
+      <c r="H20" s="40" t="s">
+        <v>207</v>
+      </c>
+      <c r="I20" s="44"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
@@ -1894,10 +1878,10 @@
         <v>52</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
@@ -1914,10 +1898,10 @@
         <v>53</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
@@ -1948,31 +1932,31 @@
         <v>51</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="E25" s="40" t="s">
-        <v>196</v>
-      </c>
-      <c r="F25" s="40"/>
-      <c r="H25" s="4" t="s">
-        <v>214</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>214</v>
+      <c r="B25" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="F25" s="10"/>
+      <c r="H25" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -2072,73 +2056,67 @@
         <v>9</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B32" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="C32" s="39" t="s">
-        <v>203</v>
-      </c>
-      <c r="E32" s="40"/>
-      <c r="F32" s="40"/>
-      <c r="H32" s="4" t="s">
+      <c r="B32" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="C32" s="13"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="H32" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="I32" s="4" t="s">
+      <c r="I32" s="9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="4" t="s">
+    <row r="33" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="C33" s="39" t="s">
-        <v>203</v>
-      </c>
-      <c r="E33" s="40"/>
-      <c r="F33" s="40"/>
-      <c r="H33" s="4">
+      <c r="B33" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="C33" s="13"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="H33" s="9">
         <v>48</v>
       </c>
-      <c r="I33" s="4">
+      <c r="I33" s="9">
         <v>48</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="4" t="s">
+    <row r="34" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="C34" s="39" t="s">
-        <v>203</v>
-      </c>
-      <c r="E34" s="40"/>
-      <c r="F34" s="40"/>
-      <c r="H34" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="I34" s="4" t="s">
-        <v>222</v>
+      <c r="B34" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C34" s="13"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="H34" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
@@ -2175,37 +2153,37 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="11" t="s">
+    <row r="37" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="C37" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="H37" s="11" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" s="39" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="39" t="s">
-        <v>198</v>
-      </c>
-      <c r="C38" s="39" t="s">
-        <v>199</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="H38" s="39" t="s">
-        <v>216</v>
-      </c>
-      <c r="I38" s="39" t="s">
-        <v>216</v>
+      <c r="B37" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="E37" s="10"/>
+      <c r="F37" s="10"/>
+      <c r="H37" s="9" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="I38" s="13" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -2284,17 +2262,17 @@
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="4" t="s">
+    <row r="43" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="E43" s="40"/>
-      <c r="F43" s="40"/>
-      <c r="H43" s="4" t="s">
-        <v>223</v>
+      <c r="B43" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="E43" s="10"/>
+      <c r="F43" s="10"/>
+      <c r="H43" s="9" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -2305,66 +2283,69 @@
         <v>47</v>
       </c>
       <c r="C44" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="E44" s="35"/>
+      <c r="F44" s="35"/>
+      <c r="H44" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+    </row>
+    <row r="46" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C46" s="13"/>
+      <c r="E46" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="F46" s="10"/>
+      <c r="H46" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="I46" s="9" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="C47" s="13"/>
+      <c r="E47" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="E44" s="40"/>
-      <c r="F44" s="40"/>
-      <c r="H44" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="I44" s="4" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-    </row>
-    <row r="46" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="39" t="s">
-        <v>202</v>
-      </c>
-      <c r="C46" s="39" t="s">
-        <v>199</v>
-      </c>
-      <c r="E46" s="40" t="s">
-        <v>206</v>
-      </c>
-      <c r="F46" s="40"/>
-      <c r="H46" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="I46" s="4" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C47" s="39" t="s">
-        <v>203</v>
-      </c>
-      <c r="E47" s="40" t="s">
-        <v>207</v>
-      </c>
-      <c r="F47" s="40"/>
-      <c r="H47" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="I47" s="4" t="s">
-        <v>219</v>
+      <c r="F47" s="10"/>
+      <c r="H47" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="I47" s="9" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2372,8 +2353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5113F5DD-FFF9-4DD1-8866-48A257EC0332}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2503,7 +2484,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>184</v>
@@ -2528,20 +2509,20 @@
         <v>107</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="5" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -2550,12 +2531,12 @@
         <v>5</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D10" s="9"/>
       <c r="F10" s="5"/>
       <c r="I10" s="3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -2574,10 +2555,10 @@
         <v>64</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.35">
@@ -2599,7 +2580,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>103</v>
@@ -2613,10 +2594,10 @@
         <v>65</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.35">
@@ -2646,8 +2627,8 @@
       <c r="C15" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
     </row>
     <row r="16" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B16" s="7" t="s">
@@ -2659,50 +2640,44 @@
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="C17" s="39" t="s">
-        <v>203</v>
-      </c>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-    </row>
-    <row r="18" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="4" t="s">
+      <c r="B17" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+    </row>
+    <row r="18" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="C18" s="39" t="s">
-        <v>203</v>
-      </c>
-      <c r="E18" s="40" t="s">
+      <c r="B18" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="E18" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="F18" s="40" t="s">
+      <c r="F18" s="10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="C19" s="39" t="s">
-        <v>203</v>
-      </c>
-      <c r="E19" s="40" t="s">
+      <c r="B19" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C19" s="13"/>
+      <c r="E19" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="F19" s="40" t="s">
+      <c r="F19" s="10" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2712,7 +2687,7 @@
         <v>104</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="10"/>
@@ -2720,15 +2695,15 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="11" t="s">
+    <row r="21" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
+      <c r="B21" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="9" t="s">
@@ -2769,10 +2744,10 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>81</v>
@@ -2785,18 +2760,18 @@
         <v>77</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>81</v>
@@ -2809,10 +2784,10 @@
         <v>78</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -2944,8 +2919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B945AFE6-1F03-45E2-947C-33FC1DE5D955}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2989,16 +2964,16 @@
         <v>115</v>
       </c>
       <c r="C2" s="15"/>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="24" t="s">
         <v>1</v>
       </c>
     </row>
@@ -3077,7 +3052,7 @@
       <c r="B9" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="33" t="s">
         <v>185</v>
       </c>
       <c r="D9" s="7"/>
@@ -3171,10 +3146,10 @@
       <c r="C15" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="E15" s="40" t="s">
+      <c r="E15" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="F15" s="40" t="s">
+      <c r="F15" s="35" t="s">
         <v>141</v>
       </c>
     </row>
@@ -3219,10 +3194,10 @@
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
-      <c r="E18" s="28" t="s">
+      <c r="E18" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="F18" s="28" t="s">
+      <c r="F18" s="25" t="s">
         <v>145</v>
       </c>
     </row>
@@ -3254,8 +3229,8 @@
         <v>110</v>
       </c>
       <c r="H20" s="16"/>
-      <c r="I20" s="41" t="s">
-        <v>211</v>
+      <c r="I20" s="36" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
@@ -3265,7 +3240,7 @@
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
-      <c r="F21" s="29"/>
+      <c r="F21" s="26"/>
       <c r="H21" s="20"/>
       <c r="I21" s="21"/>
     </row>
@@ -3279,7 +3254,7 @@
       <c r="E22" s="5">
         <v>3</v>
       </c>
-      <c r="F22" s="30"/>
+      <c r="F22" s="27"/>
       <c r="H22" s="20"/>
       <c r="I22" s="21"/>
     </row>
@@ -3290,23 +3265,20 @@
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
-      <c r="F23" s="29"/>
+      <c r="F23" s="26"/>
       <c r="H23" s="20"/>
       <c r="I23" s="21"/>
     </row>
-    <row r="24" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="42" t="s">
+    <row r="24" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="37" t="s">
         <v>193</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="E24" s="40"/>
-      <c r="F24" s="43"/>
-      <c r="H24" s="20" t="s">
-        <v>209</v>
-      </c>
-      <c r="I24" s="21"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="38"/>
+      <c r="H24" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="I24" s="39"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="20" t="s">
@@ -3318,7 +3290,7 @@
       <c r="E25" s="5">
         <v>10</v>
       </c>
-      <c r="F25" s="29"/>
+      <c r="F25" s="26"/>
       <c r="H25" s="20"/>
       <c r="I25" s="21"/>
     </row>
@@ -3329,7 +3301,7 @@
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
-      <c r="F26" s="29"/>
+      <c r="F26" s="26"/>
       <c r="H26" s="20"/>
       <c r="I26" s="21"/>
     </row>
@@ -3343,7 +3315,7 @@
       <c r="E27" s="5">
         <v>12</v>
       </c>
-      <c r="F27" s="29"/>
+      <c r="F27" s="26"/>
       <c r="H27" s="20"/>
       <c r="I27" s="21"/>
     </row>
@@ -3354,25 +3326,23 @@
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
-      <c r="F28" s="29"/>
+      <c r="F28" s="26"/>
       <c r="H28" s="20"/>
       <c r="I28" s="21"/>
     </row>
-    <row r="29" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="44" t="s">
+    <row r="29" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="40" t="s">
         <v>192</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45" t="s">
-        <v>194</v>
-      </c>
-      <c r="D29" s="45"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="47"/>
-      <c r="H29" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="I29" s="25"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="43"/>
+      <c r="H29" s="40" t="s">
+        <v>207</v>
+      </c>
+      <c r="I29" s="44"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
@@ -3422,18 +3392,15 @@
         <v>156</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="4" t="s">
+    <row r="33" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="E33" s="40"/>
-      <c r="F33" s="40"/>
+      <c r="B33" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
     </row>
     <row r="34" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
@@ -3487,11 +3454,11 @@
         <v>92</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="F37" s="12"/>
       <c r="H37" s="11" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -3511,21 +3478,21 @@
       </c>
     </row>
     <row r="39" spans="1:9" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A39" s="39" t="s">
+      <c r="A39" s="34" t="s">
         <v>127</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="E39" s="40" t="s">
+        <v>242</v>
+      </c>
+      <c r="E39" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="F39" s="40"/>
+      <c r="F39" s="35"/>
       <c r="H39" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
@@ -3543,13 +3510,13 @@
         <v>163</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="I42" s="5" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -3569,17 +3536,17 @@
     </row>
     <row r="44" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B44" s="4" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="E44" s="40"/>
-      <c r="F44" s="40" t="s">
-        <v>244</v>
-      </c>
-      <c r="I44" s="40" t="s">
-        <v>244</v>
+      <c r="E44" s="35"/>
+      <c r="F44" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="I44" s="35" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
@@ -3592,12 +3559,12 @@
       <c r="D45" s="7"/>
       <c r="E45" s="8"/>
       <c r="F45" s="8" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="G45" s="7"/>
       <c r="H45" s="7"/>
       <c r="I45" s="8" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -3612,8 +3579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D9F3751-E89E-4D65-AA53-4C5E240F65D4}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3748,7 +3715,7 @@
       <c r="B9" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="33" t="s">
         <v>185</v>
       </c>
       <c r="D9" s="7"/>
@@ -3757,7 +3724,7 @@
         <v>187</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -3911,16 +3878,16 @@
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
-      <c r="E18" s="28" t="s">
+      <c r="E18" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="F18" s="28" t="s">
+      <c r="F18" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="H18" s="28" t="s">
+      <c r="H18" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="I18" s="28" t="s">
+      <c r="I18" s="25" t="s">
         <v>145</v>
       </c>
     </row>
@@ -3951,8 +3918,8 @@
         <v>110</v>
       </c>
       <c r="H20" s="16"/>
-      <c r="I20" s="41" t="s">
-        <v>211</v>
+      <c r="I20" s="36" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
@@ -3991,19 +3958,16 @@
       <c r="H23" s="20"/>
       <c r="I23" s="21"/>
     </row>
-    <row r="24" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="42" t="s">
+    <row r="24" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="37" t="s">
         <v>193</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="E24" s="40"/>
-      <c r="F24" s="49"/>
-      <c r="H24" s="20" t="s">
-        <v>209</v>
-      </c>
-      <c r="I24" s="21"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="39"/>
+      <c r="H24" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="I24" s="39"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="20" t="s">
@@ -4055,21 +4019,19 @@
       <c r="H28" s="20"/>
       <c r="I28" s="21"/>
     </row>
-    <row r="29" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="44" t="s">
+    <row r="29" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="40" t="s">
         <v>192</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45" t="s">
-        <v>194</v>
-      </c>
-      <c r="D29" s="45"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="48"/>
-      <c r="H29" s="23" t="s">
-        <v>210</v>
-      </c>
-      <c r="I29" s="25"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="44"/>
+      <c r="H29" s="40" t="s">
+        <v>207</v>
+      </c>
+      <c r="I29" s="44"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
@@ -4119,20 +4081,17 @@
         <v>156</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="4" t="s">
+    <row r="33" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="E33" s="40"/>
-      <c r="F33" s="40"/>
-      <c r="H33" s="4" t="s">
-        <v>214</v>
+      <c r="B33" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="H33" s="9" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -4191,7 +4150,7 @@
       </c>
       <c r="F37" s="12"/>
       <c r="H37" s="11" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -4260,10 +4219,10 @@
         <v>176</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="7" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
@@ -4278,22 +4237,22 @@
         <v>55</v>
       </c>
       <c r="I42" s="8" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B43" s="4" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="E43" s="40"/>
+      <c r="E43" s="35"/>
       <c r="F43" s="4" t="s">
         <v>176</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
@@ -4307,7 +4266,7 @@
         <v>176</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -4346,7 +4305,7 @@
       <c r="C1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="37"/>
+      <c r="D1" s="32"/>
       <c r="E1" s="1" t="s">
         <v>48</v>
       </c>
@@ -4419,7 +4378,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="23" t="s">
         <v>125</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -4455,7 +4414,7 @@
       <c r="B9" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="33" t="s">
         <v>185</v>
       </c>
       <c r="D9" s="7"/>
@@ -4469,7 +4428,7 @@
       <c r="B10" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="38"/>
+      <c r="C10" s="33"/>
       <c r="D10" s="7"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8" t="s">
@@ -4516,10 +4475,10 @@
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="5" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -4536,14 +4495,14 @@
     </row>
     <row r="15" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40" t="s">
-        <v>253</v>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -4556,7 +4515,7 @@
       <c r="D16" s="7"/>
       <c r="E16" s="8"/>
       <c r="F16" s="5" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -4692,7 +4651,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="44.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.54296875" style="36" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" style="31" customWidth="1"/>
     <col min="3" max="3" width="47.90625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4700,7 +4659,7 @@
       <c r="A1" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="30" t="s">
         <v>121</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -4711,7 +4670,7 @@
       <c r="A3" t="s">
         <v>168</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="31" t="s">
         <v>164</v>
       </c>
     </row>
@@ -4719,15 +4678,15 @@
       <c r="A4" t="s">
         <v>159</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="31" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="31" t="s">
         <v>164</v>
       </c>
     </row>
@@ -4735,7 +4694,7 @@
       <c r="A6" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="31" t="s">
         <v>164</v>
       </c>
       <c r="C6" t="s">
@@ -4746,7 +4705,7 @@
       <c r="A7" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="31" t="s">
         <v>164</v>
       </c>
     </row>
@@ -4754,7 +4713,7 @@
       <c r="A8" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="31" t="s">
         <v>164</v>
       </c>
     </row>
@@ -4762,7 +4721,7 @@
       <c r="A9" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="31" t="s">
         <v>164</v>
       </c>
     </row>
@@ -4770,7 +4729,7 @@
       <c r="A11" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="31" t="s">
         <v>164</v>
       </c>
       <c r="C11" t="s">
@@ -4781,7 +4740,7 @@
       <c r="A12" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="31" t="s">
         <v>164</v>
       </c>
       <c r="C12" t="s">

</xml_diff>

<commit_message>
Moved Mappings folders and tests
</commit_message>
<xml_diff>
--- a/docs/data-maps/sam-silver-attr-map.xlsx
+++ b/docs/data-maps/sam-silver-attr-map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\defra\ls-keeper-data-api\docs\data-maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06EA7787-16B7-402B-BE67-26BF5EBE1AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302925E5-9893-4894-A6FD-2B5E19DA1B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-40" yWindow="5600" windowWidth="24250" windowHeight="15280" activeTab="1" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
+    <workbookView xWindow="14640" yWindow="4260" windowWidth="22410" windowHeight="15990" activeTab="6" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
   </bookViews>
   <sheets>
     <sheet name="SAM CPHHolding" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="SAM Party" sheetId="3" r:id="rId4"/>
     <sheet name="Party Roles" sheetId="6" r:id="rId5"/>
     <sheet name="LOVs Required" sheetId="5" r:id="rId6"/>
+    <sheet name="TODOs" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -126,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="270">
   <si>
     <t>Source</t>
   </si>
@@ -701,9 +702,6 @@
     <t>Reference data table mentioned but can see where this comes from? TBC</t>
   </si>
   <si>
-    <t>Is this either an ORG or a Person?</t>
-  </si>
-  <si>
     <t>PAON_DESCRIPTION</t>
   </si>
   <si>
@@ -869,12 +867,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>Roles[].RoleTypeCode</t>
-  </si>
-  <si>
-    <t>RoleTypeCode</t>
-  </si>
-  <si>
     <t>LIVESTOCKOWNER</t>
   </si>
   <si>
@@ -906,13 +898,52 @@
   </si>
   <si>
     <t>ProductionUsageCodeList</t>
+  </si>
+  <si>
+    <t>Multiple silver holdings</t>
+  </si>
+  <si>
+    <t>Manage holders differently vs CPHS</t>
+  </si>
+  <si>
+    <t>PartyInitials</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Holding composite keys</t>
+  </si>
+  <si>
+    <t>Holder composite keys</t>
+  </si>
+  <si>
+    <t>Party composite keys</t>
+  </si>
+  <si>
+    <t>Herd composite keys</t>
+  </si>
+  <si>
+    <t>IsHolder</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>Add created Date GOLD</t>
+  </si>
+  <si>
+    <t>Add json properties</t>
+  </si>
+  <si>
+    <t>Move upsert methods into shared service</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -992,6 +1023,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1124,7 +1162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1252,6 +1290,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1568,8 +1607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C5EF1DC-D2AC-4A4B-82BB-D60D1A15ED0A}">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1714,7 +1753,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>11</v>
@@ -1726,10 +1765,10 @@
         <v>59</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -1771,7 +1810,7 @@
       </c>
       <c r="H11" s="16"/>
       <c r="I11" s="36" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -1803,12 +1842,12 @@
     </row>
     <row r="15" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="37" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="38"/>
       <c r="H15" s="37" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I15" s="39"/>
     </row>
@@ -1852,7 +1891,7 @@
     </row>
     <row r="20" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="40" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B20" s="41"/>
       <c r="C20" s="41"/>
@@ -1860,7 +1899,7 @@
       <c r="E20" s="42"/>
       <c r="F20" s="43"/>
       <c r="H20" s="40" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I20" s="44"/>
     </row>
@@ -1878,10 +1917,10 @@
         <v>52</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
@@ -1898,10 +1937,10 @@
         <v>53</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
@@ -1932,10 +1971,10 @@
         <v>51</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
@@ -1943,20 +1982,20 @@
         <v>93</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F25" s="10"/>
       <c r="H25" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -2056,16 +2095,16 @@
         <v>9</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
@@ -2073,7 +2112,7 @@
         <v>98</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C32" s="13"/>
       <c r="E32" s="10"/>
@@ -2090,7 +2129,7 @@
         <v>66</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C33" s="13"/>
       <c r="E33" s="10"/>
@@ -2107,16 +2146,16 @@
         <v>67</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C34" s="13"/>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
       <c r="H34" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I34" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
@@ -2158,32 +2197,32 @@
         <v>182</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
       <c r="H37" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I38" s="13" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -2267,12 +2306,12 @@
         <v>183</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
       <c r="H43" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -2283,15 +2322,15 @@
         <v>47</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E44" s="35"/>
       <c r="F44" s="35"/>
       <c r="H44" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
@@ -2299,28 +2338,28 @@
         <v>99</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
     </row>
     <row r="46" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="13" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B46" s="9" t="s">
         <v>100</v>
       </c>
       <c r="C46" s="13"/>
       <c r="E46" s="10" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F46" s="10"/>
       <c r="H46" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I46" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="47" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
@@ -2328,18 +2367,18 @@
         <v>35</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C47" s="13"/>
       <c r="E47" s="10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F47" s="10"/>
       <c r="H47" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I47" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
@@ -2353,8 +2392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5113F5DD-FFF9-4DD1-8866-48A257EC0332}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2484,7 +2523,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>184</v>
@@ -2509,20 +2548,20 @@
         <v>107</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -2531,12 +2570,12 @@
         <v>5</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D10" s="9"/>
       <c r="F10" s="5"/>
       <c r="I10" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -2555,10 +2594,10 @@
         <v>64</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="17" customHeight="1" x14ac:dyDescent="0.35">
@@ -2580,7 +2619,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>103</v>
@@ -2594,10 +2633,10 @@
         <v>65</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.35">
@@ -2645,7 +2684,7 @@
         <v>98</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C17" s="13"/>
       <c r="E17" s="10"/>
@@ -2656,7 +2695,7 @@
         <v>66</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C18" s="13"/>
       <c r="E18" s="10" t="s">
@@ -2671,7 +2710,7 @@
         <v>67</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C19" s="13"/>
       <c r="E19" s="10" t="s">
@@ -2687,7 +2726,7 @@
         <v>104</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="10"/>
@@ -2700,7 +2739,7 @@
         <v>99</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -2744,10 +2783,10 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>81</v>
@@ -2760,18 +2799,18 @@
         <v>77</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>81</v>
@@ -2784,10 +2823,10 @@
         <v>78</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -2920,7 +2959,7 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2992,7 +3031,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
         <v>96</v>
       </c>
@@ -3004,100 +3043,94 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="F6" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="13" t="s">
+    <row r="9" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B9" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F9" s="10" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="7" t="s">
+    <row r="10" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C10" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8" t="s">
+      <c r="D10" s="7"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8" t="s">
         <v>186</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>131</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>142</v>
+        <v>137</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>130</v>
@@ -3107,446 +3140,450 @@
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="10" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
+    <row r="14" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="9" t="s">
+      <c r="B14" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B15" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="10" t="s">
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F15" s="5" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
+    <row r="16" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B16" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="E15" s="35" t="s">
+      <c r="E16" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="F15" s="35" t="s">
+      <c r="F16" s="10" t="s">
         <v>141</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
-      <c r="E18" s="25" t="s">
+      <c r="E18" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="F18" s="25" t="s">
+      <c r="F19" s="25" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="11" t="s">
+    <row r="20" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C20" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="16" t="s">
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B21" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C21" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="18">
+      <c r="D21" s="17"/>
+      <c r="E21" s="18">
         <v>1</v>
       </c>
-      <c r="F20" s="19" t="s">
+      <c r="F21" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="H20" s="16"/>
-      <c r="I20" s="36" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="20" t="s">
+      <c r="H21" s="16"/>
+      <c r="I21" s="36" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="20" t="s">
         <v>70</v>
-      </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="F21" s="26"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="21"/>
-    </row>
-    <row r="22" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="20" t="s">
-        <v>36</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
-      <c r="E22" s="5">
-        <v>3</v>
-      </c>
-      <c r="F22" s="27"/>
+      <c r="F22" s="26"/>
       <c r="H22" s="20"/>
       <c r="I22" s="21"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="20" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
-      <c r="F23" s="26"/>
+      <c r="E23" s="5">
+        <v>3</v>
+      </c>
+      <c r="F23" s="27"/>
       <c r="H23" s="20"/>
       <c r="I23" s="21"/>
     </row>
-    <row r="24" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="37" t="s">
-        <v>193</v>
-      </c>
-      <c r="E24" s="10"/>
-      <c r="F24" s="38"/>
-      <c r="H24" s="37" t="s">
-        <v>206</v>
-      </c>
-      <c r="I24" s="39"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="5">
-        <v>10</v>
-      </c>
-      <c r="F25" s="26"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="21"/>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="F24" s="26"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="21"/>
+    </row>
+    <row r="25" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25" s="38"/>
+      <c r="H25" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="I25" s="39"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="20" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
+      <c r="E26" s="5">
+        <v>10</v>
+      </c>
       <c r="F26" s="26"/>
       <c r="H26" s="20"/>
       <c r="I26" s="21"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="20" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
-      <c r="E27" s="5">
-        <v>12</v>
-      </c>
       <c r="F27" s="26"/>
       <c r="H27" s="20"/>
       <c r="I27" s="21"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="20" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
+      <c r="E28" s="5">
+        <v>12</v>
+      </c>
       <c r="F28" s="26"/>
       <c r="H28" s="20"/>
       <c r="I28" s="21"/>
     </row>
-    <row r="29" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="40" t="s">
-        <v>192</v>
-      </c>
-      <c r="B29" s="41"/>
-      <c r="C29" s="41"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="42"/>
-      <c r="F29" s="43"/>
-      <c r="H29" s="40" t="s">
-        <v>207</v>
-      </c>
-      <c r="I29" s="44"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>158</v>
-      </c>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="F29" s="26"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="21"/>
+    </row>
+    <row r="30" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="B30" s="41"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="43"/>
+      <c r="H30" s="40" t="s">
+        <v>206</v>
+      </c>
+      <c r="I30" s="44"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
       <c r="E31" s="10" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
       <c r="E32" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="F33" s="10" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="9" t="s">
+    <row r="34" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B33" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-    </row>
-    <row r="34" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="3" t="s">
+      <c r="B34" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+    </row>
+    <row r="35" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="F34" s="10" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A35" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>152</v>
       </c>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
       <c r="E35" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="F36" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="7" t="s">
+    <row r="37" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C37" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8" t="s">
+      <c r="E37" s="8"/>
+      <c r="F37" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="11" t="s">
+    <row r="38" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C38" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="E37" s="12" t="s">
+      <c r="E38" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="F38" s="12"/>
+      <c r="H38" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="F37" s="12"/>
-      <c r="H37" s="11" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="9" t="s">
+    </row>
+    <row r="39" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B39" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="5">
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="5">
         <v>25962203</v>
       </c>
-      <c r="F38" s="5">
+      <c r="F39" s="5">
         <v>25962203</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A39" s="34" t="s">
+    <row r="40" spans="1:9" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+      <c r="A40" s="34" t="s">
         <v>127</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B40" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="E39" s="35" t="s">
+      <c r="C40" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="E40" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="F39" s="35"/>
-      <c r="H39" s="4" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="B40" s="9" t="s">
-        <v>160</v>
+      <c r="F40" s="35"/>
+      <c r="H40" s="4" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B41" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B42" s="9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B43" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C43" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="F43" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="F42" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="I42" s="5" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="7" t="s">
+      <c r="I43" s="5" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C44" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8" t="s">
+      <c r="E44" s="8"/>
+      <c r="F44" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="I43" s="8" t="s">
+      <c r="I44" s="8" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="E44" s="35"/>
-      <c r="F44" s="35" t="s">
-        <v>240</v>
-      </c>
-      <c r="I44" s="35" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
@@ -3559,18 +3596,18 @@
       <c r="D45" s="7"/>
       <c r="E45" s="8"/>
       <c r="F45" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G45" s="7"/>
       <c r="H45" s="7"/>
       <c r="I45" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="E6 E17:F17" numberStoredAsText="1"/>
+    <ignoredError sqref="E7 E18:F18" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -3580,7 +3617,7 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3654,116 +3691,110 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+      <c r="B6" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
       <c r="E7" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F8" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I8" s="10" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="13" t="s">
+    <row r="9" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B9" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="E8" s="10" t="s">
+      <c r="C9" s="13"/>
+      <c r="E9" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F9" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H9" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I9" s="10" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="13"/>
-      <c r="B9" s="7" t="s">
+    <row r="10" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="13"/>
+      <c r="B10" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C10" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8" t="s">
+      <c r="D10" s="7"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="I9" s="8" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>137</v>
+      <c r="I10" s="8" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>131</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>142</v>
+        <v>137</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>130</v>
@@ -3773,486 +3804,493 @@
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D13" s="9"/>
+      <c r="E13" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="9" t="s">
-        <v>86</v>
-      </c>
       <c r="B14" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
+        <v>259</v>
+      </c>
       <c r="E14" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>140</v>
+        <v>260</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
       <c r="E15" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>134</v>
+        <v>87</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>133</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
-      <c r="E16" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>143</v>
+      <c r="E16" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
-      <c r="E18" s="25" t="s">
+      <c r="E18" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="F18" s="25" t="s">
+      <c r="F19" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="H18" s="25" t="s">
+      <c r="H19" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="I18" s="25" t="s">
+      <c r="I19" s="25" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="11" t="s">
+    <row r="20" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C20" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="E19" s="12"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" s="16" t="s">
+      <c r="E20" s="12"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B21" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="C21" s="17" t="s">
         <v>151</v>
       </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="18">
+      <c r="D21" s="17"/>
+      <c r="E21" s="18">
         <v>1</v>
       </c>
-      <c r="F20" s="19" t="s">
+      <c r="F21" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="H20" s="16"/>
-      <c r="I20" s="36" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="20" t="s">
+      <c r="H21" s="16"/>
+      <c r="I21" s="36" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="20" t="s">
         <v>70</v>
-      </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="F21" s="21"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="21"/>
-    </row>
-    <row r="22" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="20" t="s">
-        <v>36</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
-      <c r="E22" s="5">
-        <v>3</v>
-      </c>
-      <c r="F22" s="22"/>
+      <c r="F22" s="21"/>
       <c r="H22" s="20"/>
       <c r="I22" s="21"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="20" t="s">
-        <v>71</v>
+        <v>36</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
-      <c r="F23" s="21"/>
+      <c r="E23" s="5">
+        <v>3</v>
+      </c>
+      <c r="F23" s="22"/>
       <c r="H23" s="20"/>
       <c r="I23" s="21"/>
     </row>
-    <row r="24" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="37" t="s">
-        <v>193</v>
-      </c>
-      <c r="E24" s="10"/>
-      <c r="F24" s="39"/>
-      <c r="H24" s="37" t="s">
-        <v>206</v>
-      </c>
-      <c r="I24" s="39"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="5">
-        <v>10</v>
-      </c>
-      <c r="F25" s="21"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="21"/>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="F24" s="21"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="21"/>
+    </row>
+    <row r="25" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25" s="39"/>
+      <c r="H25" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="I25" s="39"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="20" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
+      <c r="E26" s="5">
+        <v>10</v>
+      </c>
       <c r="F26" s="21"/>
       <c r="H26" s="20"/>
       <c r="I26" s="21"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="20" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
-      <c r="E27" s="5">
-        <v>12</v>
-      </c>
       <c r="F27" s="21"/>
       <c r="H27" s="20"/>
       <c r="I27" s="21"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="20" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
+      <c r="E28" s="5">
+        <v>12</v>
+      </c>
       <c r="F28" s="21"/>
       <c r="H28" s="20"/>
       <c r="I28" s="21"/>
     </row>
-    <row r="29" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="40" t="s">
-        <v>192</v>
-      </c>
-      <c r="B29" s="41"/>
-      <c r="C29" s="41"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="42"/>
-      <c r="F29" s="44"/>
-      <c r="H29" s="40" t="s">
-        <v>207</v>
-      </c>
-      <c r="I29" s="44"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>158</v>
-      </c>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="F29" s="21"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="21"/>
+    </row>
+    <row r="30" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="B30" s="41"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="44"/>
+      <c r="H30" s="40" t="s">
+        <v>206</v>
+      </c>
+      <c r="I30" s="44"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
       <c r="E31" s="10" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
       <c r="E32" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="F33" s="10" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="9" t="s">
+    <row r="34" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="B33" s="9" t="s">
-        <v>243</v>
-      </c>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="H33" s="9" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="3" t="s">
+      <c r="B34" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="H34" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="F34" s="10" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A35" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>152</v>
       </c>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
       <c r="E35" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="F35" s="5" t="s">
+      <c r="F36" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="7" t="s">
+    <row r="37" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C37" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8" t="s">
+      <c r="E37" s="8"/>
+      <c r="F37" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="11" t="s">
+    <row r="38" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C38" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="E37" s="12" t="s">
+      <c r="E38" s="12" t="s">
         <v>164</v>
       </c>
-      <c r="F37" s="12"/>
-      <c r="H37" s="11" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="9" t="s">
+      <c r="F38" s="12"/>
+      <c r="H38" s="11" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B39" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="5">
+      <c r="C39" s="9"/>
+      <c r="D39" s="9"/>
+      <c r="E39" s="5">
         <v>25962203</v>
       </c>
-      <c r="F38" s="5">
+      <c r="F39" s="5">
         <v>25962203</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A39" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B41" s="9" t="s">
         <v>161</v>
-      </c>
-      <c r="C40" s="9"/>
-      <c r="E40" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A41" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>163</v>
       </c>
       <c r="C41" s="9"/>
       <c r="E41" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="C42" s="9"/>
+      <c r="E42" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="F42" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="H41" s="3" t="s">
-        <v>251</v>
-      </c>
-      <c r="I41" s="3" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" s="7" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B42" s="7" t="s">
+      <c r="H42" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" s="7" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B43" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C43" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8" t="s">
+      <c r="E43" s="8"/>
+      <c r="F43" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="I42" s="8" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="E43" s="35"/>
-      <c r="F43" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>251</v>
+      <c r="I43" s="8" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
@@ -4266,13 +4304,13 @@
         <v>176</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="E6:F6 E17:F17 H17:I17 I6" numberStoredAsText="1"/>
+    <ignoredError sqref="E7:F7 E18:F18 H18:I18 I7" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -4282,7 +4320,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4436,73 +4474,73 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>57</v>
+      <c r="A11" s="9"/>
+      <c r="B11" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="C11" s="33"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="C12" s="9"/>
+        <v>171</v>
+      </c>
       <c r="D12" s="9"/>
       <c r="E12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="B13" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>174</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="C13" s="9"/>
       <c r="D13" s="9"/>
       <c r="E13" s="5" t="s">
-        <v>249</v>
+        <v>58</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B14" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="D14" s="9"/>
+      <c r="E14" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C15" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8" t="s">
+      <c r="E15" s="8"/>
+      <c r="F15" s="8" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -4515,7 +4553,7 @@
       <c r="D16" s="7"/>
       <c r="E16" s="8"/>
       <c r="F16" s="5" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -4751,4 +4789,64 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4719B872-65ED-4B8C-BD24-70C5594D80D1}">
+  <dimension ref="A2:A11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="46" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="45" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="45" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="45" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="45" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="45" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" s="29" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>269</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
CTS and SAM Silver steps completed
</commit_message>
<xml_diff>
--- a/docs/data-maps/sam-silver-attr-map.xlsx
+++ b/docs/data-maps/sam-silver-attr-map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\defra\ls-keeper-data-api\docs\data-maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302925E5-9893-4894-A6FD-2B5E19DA1B5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B3C779-4A03-4C27-8A8D-21E349937B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14640" yWindow="4260" windowWidth="22410" windowHeight="15990" activeTab="6" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
+    <workbookView xWindow="14640" yWindow="4260" windowWidth="22410" windowHeight="15990" activeTab="4" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
   </bookViews>
   <sheets>
     <sheet name="SAM CPHHolding" sheetId="1" r:id="rId1"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="268">
   <si>
     <t>Source</t>
   </si>
@@ -852,9 +852,6 @@
     <t>CPH Holder</t>
   </si>
   <si>
-    <t>Parsed set of CPH's. Check if we can make this work better to avoid repeat calls and this needs removing from the Party but including in the relationship doc.</t>
-  </si>
-  <si>
     <t>Address.CountrySubDivision</t>
   </si>
   <si>
@@ -933,17 +930,14 @@
     <t>Add created Date GOLD</t>
   </si>
   <si>
-    <t>Add json properties</t>
-  </si>
-  <si>
-    <t>Move upsert methods into shared service</t>
+    <t>Check all gold documents e.g. reference type keys not full objects</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1018,14 +1012,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1162,7 +1148,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1257,9 +1243,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1290,7 +1273,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1809,7 +1792,7 @@
         <v>110</v>
       </c>
       <c r="H11" s="16"/>
-      <c r="I11" s="36" t="s">
+      <c r="I11" s="35" t="s">
         <v>207</v>
       </c>
     </row>
@@ -1841,15 +1824,15 @@
       <c r="I14" s="21"/>
     </row>
     <row r="15" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="37" t="s">
+      <c r="A15" s="36" t="s">
         <v>192</v>
       </c>
       <c r="E15" s="10"/>
-      <c r="F15" s="38"/>
-      <c r="H15" s="37" t="s">
+      <c r="F15" s="37"/>
+      <c r="H15" s="36" t="s">
         <v>205</v>
       </c>
-      <c r="I15" s="39"/>
+      <c r="I15" s="38"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="20" t="s">
@@ -1890,18 +1873,18 @@
       <c r="I19" s="21"/>
     </row>
     <row r="20" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="40" t="s">
+      <c r="A20" s="39" t="s">
         <v>191</v>
       </c>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="43"/>
-      <c r="H20" s="40" t="s">
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="42"/>
+      <c r="H20" s="39" t="s">
         <v>206</v>
       </c>
-      <c r="I20" s="44"/>
+      <c r="I20" s="43"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
@@ -2197,7 +2180,7 @@
         <v>182</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E37" s="10"/>
       <c r="F37" s="10"/>
@@ -2210,7 +2193,7 @@
         <v>196</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E38" s="10" t="s">
         <v>201</v>
@@ -2306,7 +2289,7 @@
         <v>183</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
@@ -2324,8 +2307,8 @@
       <c r="C44" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="E44" s="35"/>
-      <c r="F44" s="35"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="34"/>
       <c r="H44" s="4" t="s">
         <v>213</v>
       </c>
@@ -2338,7 +2321,7 @@
         <v>99</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
@@ -2367,7 +2350,7 @@
         <v>35</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C47" s="13"/>
       <c r="E47" s="10" t="s">
@@ -2666,8 +2649,8 @@
       <c r="C15" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
     </row>
     <row r="16" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B16" s="7" t="s">
@@ -2739,7 +2722,7 @@
         <v>99</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -2958,7 +2941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B945AFE6-1F03-45E2-947C-33FC1DE5D955}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
@@ -3045,14 +3028,14 @@
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I6" s="10" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
@@ -3166,13 +3149,13 @@
         <v>85</v>
       </c>
       <c r="B14" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="E14" s="10" t="s">
-        <v>260</v>
-      </c>
       <c r="F14" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -3281,7 +3264,7 @@
         <v>110</v>
       </c>
       <c r="H21" s="16"/>
-      <c r="I21" s="36" t="s">
+      <c r="I21" s="35" t="s">
         <v>207</v>
       </c>
     </row>
@@ -3322,15 +3305,15 @@
       <c r="I24" s="21"/>
     </row>
     <row r="25" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="37" t="s">
+      <c r="A25" s="36" t="s">
         <v>192</v>
       </c>
       <c r="E25" s="10"/>
-      <c r="F25" s="38"/>
-      <c r="H25" s="37" t="s">
+      <c r="F25" s="37"/>
+      <c r="H25" s="36" t="s">
         <v>205</v>
       </c>
-      <c r="I25" s="39"/>
+      <c r="I25" s="38"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="20" t="s">
@@ -3383,18 +3366,18 @@
       <c r="I29" s="21"/>
     </row>
     <row r="30" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="39" t="s">
         <v>191</v>
       </c>
-      <c r="B30" s="41"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="43"/>
-      <c r="H30" s="40" t="s">
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="42"/>
+      <c r="H30" s="39" t="s">
         <v>206</v>
       </c>
-      <c r="I30" s="44"/>
+      <c r="I30" s="43"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
@@ -3449,7 +3432,7 @@
         <v>93</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
@@ -3506,11 +3489,11 @@
         <v>92</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F38" s="12"/>
       <c r="H38" s="11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -3529,22 +3512,19 @@
         <v>25962203</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="4" customFormat="1" ht="58" x14ac:dyDescent="0.35">
-      <c r="A40" s="34" t="s">
+    <row r="40" spans="1:9" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A40" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="E40" s="35" t="s">
+      <c r="E40" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="F40" s="35"/>
-      <c r="H40" s="4" t="s">
-        <v>243</v>
+      <c r="F40" s="10"/>
+      <c r="H40" s="9" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
@@ -3616,8 +3596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D9F3751-E89E-4D65-AA53-4C5E240F65D4}">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3692,7 +3672,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="10" t="s">
@@ -3773,7 +3753,7 @@
         <v>187</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -3831,13 +3811,13 @@
         <v>85</v>
       </c>
       <c r="B14" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="E14" s="10" t="s">
-        <v>260</v>
-      </c>
       <c r="F14" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -3971,7 +3951,7 @@
         <v>110</v>
       </c>
       <c r="H21" s="16"/>
-      <c r="I21" s="36" t="s">
+      <c r="I21" s="35" t="s">
         <v>207</v>
       </c>
     </row>
@@ -4012,15 +3992,15 @@
       <c r="I24" s="21"/>
     </row>
     <row r="25" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="37" t="s">
+      <c r="A25" s="36" t="s">
         <v>192</v>
       </c>
       <c r="E25" s="10"/>
-      <c r="F25" s="39"/>
-      <c r="H25" s="37" t="s">
+      <c r="F25" s="38"/>
+      <c r="H25" s="36" t="s">
         <v>205</v>
       </c>
-      <c r="I25" s="39"/>
+      <c r="I25" s="38"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="20" t="s">
@@ -4073,18 +4053,18 @@
       <c r="I29" s="21"/>
     </row>
     <row r="30" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="39" t="s">
         <v>191</v>
       </c>
-      <c r="B30" s="41"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="44"/>
-      <c r="H30" s="40" t="s">
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="43"/>
+      <c r="H30" s="39" t="s">
         <v>206</v>
       </c>
-      <c r="I30" s="44"/>
+      <c r="I30" s="43"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
@@ -4139,7 +4119,7 @@
         <v>93</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E34" s="10"/>
       <c r="F34" s="10"/>
@@ -4203,7 +4183,7 @@
       </c>
       <c r="F38" s="12"/>
       <c r="H38" s="11" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -4272,10 +4252,10 @@
         <v>176</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="7" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
@@ -4290,7 +4270,7 @@
         <v>55</v>
       </c>
       <c r="I43" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
@@ -4304,7 +4284,7 @@
         <v>176</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -4319,8 +4299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91CC36E6-DB4D-4568-987C-6F2A58047854}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4476,7 +4456,7 @@
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="9"/>
       <c r="B11" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C11" s="33"/>
       <c r="D11" s="7"/>
@@ -4525,10 +4505,10 @@
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.35">
@@ -4553,7 +4533,7 @@
       <c r="D16" s="7"/>
       <c r="E16" s="8"/>
       <c r="F16" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -4793,58 +4773,59 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4719B872-65ED-4B8C-BD24-70C5594D80D1}">
-  <dimension ref="A2:A11"/>
+  <dimension ref="A2:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="46" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="58.36328125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="44" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="44" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>258</v>
-      </c>
-    </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="44" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="44" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" s="45" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="44" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" s="45" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="44" t="s">
         <v>263</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" s="45" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" s="29" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>269</v>
-      </c>
+        <v>267</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated the gold documents and domain models.
</commit_message>
<xml_diff>
--- a/docs/data-maps/sam-silver-attr-map.xlsx
+++ b/docs/data-maps/sam-silver-attr-map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\defra\ls-keeper-data-api\docs\data-maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FD4459-7553-42A4-9616-254FB6BE3819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27F7F4B-25BB-46C1-AE61-E2AA0427C16B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="1" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
+    <workbookView xWindow="1630" yWindow="2320" windowWidth="22410" windowHeight="15990" activeTab="6" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
   </bookViews>
   <sheets>
     <sheet name="SAM CPHHolding" sheetId="1" r:id="rId1"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="270">
   <si>
     <t>Source</t>
   </si>
@@ -934,6 +934,9 @@
   </si>
   <si>
     <t>SiteIdentifierType</t>
+  </si>
+  <si>
+    <t>Remove batchId from Gold</t>
   </si>
 </sst>
 </file>
@@ -2365,7 +2368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5113F5DD-FFF9-4DD1-8866-48A257EC0332}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -4773,8 +4776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4719B872-65ED-4B8C-BD24-70C5594D80D1}">
   <dimension ref="A2:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="46" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4813,17 +4816,19 @@
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" s="44" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="44" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" s="29"/>
+      <c r="A10" s="44" t="s">
+        <v>269</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update SAM silver-gold mappings (#51)
* Separate out mappings to help with future changes. Moved CTS mapping namespace.

* Updated the gold documents and domain models.

* Look to fix build errors.

---------

Co-authored-by: Mark Gent <Mark.Gent@homesengland.gov.uk>
</commit_message>
<xml_diff>
--- a/docs/data-maps/sam-silver-attr-map.xlsx
+++ b/docs/data-maps/sam-silver-attr-map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\defra\ls-keeper-data-api\docs\data-maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FD4459-7553-42A4-9616-254FB6BE3819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C27F7F4B-25BB-46C1-AE61-E2AA0427C16B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="1" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
+    <workbookView xWindow="1630" yWindow="2320" windowWidth="22410" windowHeight="15990" activeTab="6" xr2:uid="{1BA62C16-295B-4239-B5A9-F8E1565DE45D}"/>
   </bookViews>
   <sheets>
     <sheet name="SAM CPHHolding" sheetId="1" r:id="rId1"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="270">
   <si>
     <t>Source</t>
   </si>
@@ -934,6 +934,9 @@
   </si>
   <si>
     <t>SiteIdentifierType</t>
+  </si>
+  <si>
+    <t>Remove batchId from Gold</t>
   </si>
 </sst>
 </file>
@@ -2365,7 +2368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5113F5DD-FFF9-4DD1-8866-48A257EC0332}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -4773,8 +4776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4719B872-65ED-4B8C-BD24-70C5594D80D1}">
   <dimension ref="A2:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="46" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4813,17 +4816,19 @@
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" s="44" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="44" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" s="29"/>
+      <c r="A10" s="44" t="s">
+        <v>269</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>